<commit_message>
added posm count kpi
</commit_message>
<xml_diff>
--- a/Projects/JRIJP/Data/Template.xlsx
+++ b/Projects/JRIJP/Data/Template.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
   <si>
     <t xml:space="preserve">kpi_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT_POSM_PER_SCENE</t>
   </si>
   <si>
     <t xml:space="preserve">FACINGS_IN_CELL_PER_PRODUCT</t>
@@ -38,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -59,6 +62,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -75,7 +85,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -83,6 +93,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -109,12 +126,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -135,33 +156,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.9132653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the canvas kpis
</commit_message>
<xml_diff>
--- a/Projects/JRIJP/Data/Template.xlsx
+++ b/Projects/JRIJP/Data/Template.xlsx
@@ -159,13 +159,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>